<commit_message>
fixed HPO attribute (#10)
</commit_message>
<xml_diff>
--- a/emx/dist/umdm.xlsx
+++ b/emx/dist/umdm.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="775">
   <si>
     <t>umdm</t>
   </si>
@@ -682,6 +682,9 @@
     <t>biospecimenUsability</t>
   </si>
   <si>
+    <t>belongsToLabProcedure</t>
+  </si>
+  <si>
     <t>inputAmount</t>
   </si>
   <si>
@@ -712,9 +715,6 @@
     <t>sequencingID</t>
   </si>
   <si>
-    <t>belongsToLabProcedure</t>
-  </si>
-  <si>
     <t>belongsToSamplePreparation</t>
   </si>
   <si>
@@ -1510,6 +1510,9 @@
     <t>http://purl.obolibrary.org/obo/NCIT_C93400</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25294</t>
+  </si>
+  <si>
     <t>http://purl.allotrope.org/ontologies/role#AFRL_0000010</t>
   </si>
   <si>
@@ -1538,9 +1541,6 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C171337</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25294</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C69216</t>
@@ -3488,7 +3488,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L227"/>
+  <dimension ref="A1:L229"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7537,7 +7537,7 @@
         <v>221</v>
       </c>
       <c r="C121" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D121" t="b">
         <v>0</v>
@@ -7552,13 +7552,16 @@
         <v>0</v>
       </c>
       <c r="H121" t="s">
-        <v>364</v>
+        <v>67</v>
       </c>
       <c r="I121" s="2" t="s">
         <v>497</v>
       </c>
       <c r="J121" t="b">
         <v>1</v>
+      </c>
+      <c r="K121" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="122" spans="1:12">
@@ -7566,10 +7569,10 @@
         <v>139</v>
       </c>
       <c r="B122" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C122" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D122" t="b">
         <v>0</v>
@@ -7584,16 +7587,13 @@
         <v>0</v>
       </c>
       <c r="H122" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>498</v>
+        <v>483</v>
       </c>
       <c r="J122" t="b">
         <v>1</v>
-      </c>
-      <c r="K122" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="123" spans="1:12">
@@ -7601,10 +7601,10 @@
         <v>139</v>
       </c>
       <c r="B123" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C123" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D123" t="b">
         <v>0</v>
@@ -7619,10 +7619,10 @@
         <v>0</v>
       </c>
       <c r="H123" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I123" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="J123" t="b">
         <v>1</v>
@@ -7633,7 +7633,7 @@
         <v>139</v>
       </c>
       <c r="B124" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C124" t="s">
         <v>275</v>
@@ -7651,10 +7651,10 @@
         <v>0</v>
       </c>
       <c r="H124" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I124" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J124" t="b">
         <v>1</v>
@@ -7668,7 +7668,7 @@
         <v>139</v>
       </c>
       <c r="B125" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C125" t="s">
         <v>281</v>
@@ -7686,10 +7686,10 @@
         <v>0</v>
       </c>
       <c r="H125" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="J125" t="b">
         <v>1</v>
@@ -7700,10 +7700,10 @@
         <v>139</v>
       </c>
       <c r="B126" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C126" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D126" t="b">
         <v>0</v>
@@ -7718,13 +7718,16 @@
         <v>0</v>
       </c>
       <c r="H126" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I126" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J126" t="b">
         <v>1</v>
+      </c>
+      <c r="K126" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="127" spans="1:12">
@@ -7732,10 +7735,10 @@
         <v>139</v>
       </c>
       <c r="B127" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C127" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D127" t="b">
         <v>0</v>
@@ -7750,10 +7753,10 @@
         <v>0</v>
       </c>
       <c r="H127" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I127" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="J127" t="b">
         <v>1</v>
@@ -7764,10 +7767,10 @@
         <v>139</v>
       </c>
       <c r="B128" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C128" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D128" t="b">
         <v>0</v>
@@ -7782,10 +7785,10 @@
         <v>0</v>
       </c>
       <c r="H128" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I128" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J128" t="b">
         <v>1</v>
@@ -7796,10 +7799,10 @@
         <v>139</v>
       </c>
       <c r="B129" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C129" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D129" t="b">
         <v>0</v>
@@ -7814,10 +7817,10 @@
         <v>0</v>
       </c>
       <c r="H129" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I129" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J129" t="b">
         <v>1</v>
@@ -7828,10 +7831,10 @@
         <v>139</v>
       </c>
       <c r="B130" t="s">
-        <v>170</v>
+        <v>229</v>
       </c>
       <c r="C130" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D130" t="b">
         <v>0</v>
@@ -7846,16 +7849,13 @@
         <v>0</v>
       </c>
       <c r="H130" t="s">
-        <v>69</v>
+        <v>371</v>
       </c>
       <c r="I130" s="2" t="s">
-        <v>441</v>
+        <v>505</v>
       </c>
       <c r="J130" t="b">
         <v>1</v>
-      </c>
-      <c r="K130" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="131" spans="1:12">
@@ -7863,10 +7863,10 @@
         <v>139</v>
       </c>
       <c r="B131" t="s">
-        <v>171</v>
+        <v>230</v>
       </c>
       <c r="C131" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D131" t="b">
         <v>0</v>
@@ -7881,10 +7881,10 @@
         <v>0</v>
       </c>
       <c r="H131" t="s">
-        <v>310</v>
+        <v>372</v>
       </c>
       <c r="I131" s="2" t="s">
-        <v>442</v>
+        <v>506</v>
       </c>
       <c r="J131" t="b">
         <v>1</v>
@@ -7895,10 +7895,10 @@
         <v>139</v>
       </c>
       <c r="B132" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C132" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D132" t="b">
         <v>0</v>
@@ -7913,16 +7913,16 @@
         <v>0</v>
       </c>
       <c r="H132" t="s">
-        <v>311</v>
+        <v>69</v>
       </c>
       <c r="I132" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J132" t="b">
         <v>1</v>
       </c>
-      <c r="L132" t="s">
-        <v>171</v>
+      <c r="K132" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="133" spans="1:12">
@@ -7930,16 +7930,16 @@
         <v>139</v>
       </c>
       <c r="B133" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C133" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D133" t="b">
         <v>0</v>
       </c>
       <c r="E133" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F133" t="b">
         <v>0</v>
@@ -7948,16 +7948,13 @@
         <v>0</v>
       </c>
       <c r="H133" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J133" t="b">
         <v>1</v>
-      </c>
-      <c r="L133" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="134" spans="1:12">
@@ -7965,16 +7962,16 @@
         <v>139</v>
       </c>
       <c r="B134" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C134" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D134" t="b">
         <v>0</v>
       </c>
       <c r="E134" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F134" t="b">
         <v>0</v>
@@ -7983,10 +7980,10 @@
         <v>0</v>
       </c>
       <c r="H134" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J134" t="b">
         <v>1</v>
@@ -8000,7 +7997,7 @@
         <v>139</v>
       </c>
       <c r="B135" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C135" t="s">
         <v>283</v>
@@ -8009,7 +8006,7 @@
         <v>0</v>
       </c>
       <c r="E135" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F135" t="b">
         <v>0</v>
@@ -8018,10 +8015,10 @@
         <v>0</v>
       </c>
       <c r="H135" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="J135" t="b">
         <v>1</v>
@@ -8035,7 +8032,7 @@
         <v>139</v>
       </c>
       <c r="B136" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C136" t="s">
         <v>274</v>
@@ -8044,7 +8041,7 @@
         <v>0</v>
       </c>
       <c r="E136" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F136" t="b">
         <v>0</v>
@@ -8053,10 +8050,10 @@
         <v>0</v>
       </c>
       <c r="H136" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I136" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J136" t="b">
         <v>1</v>
@@ -8067,45 +8064,48 @@
     </row>
     <row r="137" spans="1:12">
       <c r="A137" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>230</v>
+        <v>175</v>
       </c>
       <c r="C137" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="D137" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F137" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G137" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H137" t="s">
-        <v>373</v>
+        <v>314</v>
       </c>
       <c r="I137" s="2" t="s">
-        <v>506</v>
+        <v>446</v>
       </c>
       <c r="J137" t="b">
         <v>1</v>
+      </c>
+      <c r="L137" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B138" t="s">
-        <v>231</v>
+        <v>176</v>
       </c>
       <c r="C138" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D138" t="b">
         <v>0</v>
@@ -8120,16 +8120,16 @@
         <v>0</v>
       </c>
       <c r="H138" t="s">
-        <v>67</v>
+        <v>315</v>
       </c>
       <c r="I138" s="2" t="s">
-        <v>507</v>
+        <v>447</v>
       </c>
       <c r="J138" t="b">
         <v>1</v>
       </c>
-      <c r="K138" t="s">
-        <v>143</v>
+      <c r="L138" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="139" spans="1:12">
@@ -8137,34 +8137,31 @@
         <v>140</v>
       </c>
       <c r="B139" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C139" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D139" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E139" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F139" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G139" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H139" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="I139" s="2" t="s">
-        <v>495</v>
+        <v>507</v>
       </c>
       <c r="J139" t="b">
         <v>1</v>
-      </c>
-      <c r="K139" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="140" spans="1:12">
@@ -8172,7 +8169,7 @@
         <v>140</v>
       </c>
       <c r="B140" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="C140" t="s">
         <v>275</v>
@@ -8190,16 +8187,16 @@
         <v>0</v>
       </c>
       <c r="H140" t="s">
-        <v>374</v>
+        <v>67</v>
       </c>
       <c r="I140" s="2" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="J140" t="b">
         <v>1</v>
       </c>
       <c r="K140" t="s">
-        <v>562</v>
+        <v>143</v>
       </c>
     </row>
     <row r="141" spans="1:12">
@@ -8207,10 +8204,10 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C141" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="D141" t="b">
         <v>0</v>
@@ -8225,13 +8222,16 @@
         <v>0</v>
       </c>
       <c r="H141" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="I141" s="2" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="J141" t="b">
         <v>1</v>
+      </c>
+      <c r="K141" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="142" spans="1:12">
@@ -8239,7 +8239,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C142" t="s">
         <v>275</v>
@@ -8257,16 +8257,16 @@
         <v>0</v>
       </c>
       <c r="H142" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="I142" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="J142" t="b">
         <v>1</v>
       </c>
       <c r="K142" t="s">
-        <v>144</v>
+        <v>562</v>
       </c>
     </row>
     <row r="143" spans="1:12">
@@ -8274,10 +8274,10 @@
         <v>140</v>
       </c>
       <c r="B143" t="s">
-        <v>42</v>
+        <v>234</v>
       </c>
       <c r="C143" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D143" t="b">
         <v>0</v>
@@ -8292,16 +8292,13 @@
         <v>0</v>
       </c>
       <c r="H143" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="I143" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="J143" t="b">
         <v>1</v>
-      </c>
-      <c r="K143" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="144" spans="1:12">
@@ -8309,7 +8306,7 @@
         <v>140</v>
       </c>
       <c r="B144" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C144" t="s">
         <v>275</v>
@@ -8327,16 +8324,16 @@
         <v>0</v>
       </c>
       <c r="H144" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I144" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="J144" t="b">
         <v>1</v>
       </c>
       <c r="K144" t="s">
-        <v>568</v>
+        <v>144</v>
       </c>
     </row>
     <row r="145" spans="1:12">
@@ -8344,7 +8341,7 @@
         <v>140</v>
       </c>
       <c r="B145" t="s">
-        <v>237</v>
+        <v>42</v>
       </c>
       <c r="C145" t="s">
         <v>275</v>
@@ -8362,16 +8359,16 @@
         <v>0</v>
       </c>
       <c r="H145" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I145" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J145" t="b">
         <v>1</v>
       </c>
       <c r="K145" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="146" spans="1:12">
@@ -8379,10 +8376,10 @@
         <v>140</v>
       </c>
       <c r="B146" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C146" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D146" t="b">
         <v>0</v>
@@ -8397,13 +8394,16 @@
         <v>0</v>
       </c>
       <c r="H146" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I146" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="J146" t="b">
         <v>1</v>
+      </c>
+      <c r="K146" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="147" spans="1:12">
@@ -8411,10 +8411,10 @@
         <v>140</v>
       </c>
       <c r="B147" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C147" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D147" t="b">
         <v>0</v>
@@ -8429,13 +8429,16 @@
         <v>0</v>
       </c>
       <c r="H147" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I147" s="2" t="s">
-        <v>503</v>
+        <v>513</v>
       </c>
       <c r="J147" t="b">
         <v>1</v>
+      </c>
+      <c r="K147" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="148" spans="1:12">
@@ -8443,7 +8446,7 @@
         <v>140</v>
       </c>
       <c r="B148" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C148" t="s">
         <v>277</v>
@@ -8461,10 +8464,10 @@
         <v>0</v>
       </c>
       <c r="H148" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="I148" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J148" t="b">
         <v>1</v>
@@ -8475,10 +8478,10 @@
         <v>140</v>
       </c>
       <c r="B149" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C149" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D149" t="b">
         <v>0</v>
@@ -8493,10 +8496,10 @@
         <v>0</v>
       </c>
       <c r="H149" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I149" s="2" t="s">
-        <v>516</v>
+        <v>504</v>
       </c>
       <c r="J149" t="b">
         <v>1</v>
@@ -8507,10 +8510,10 @@
         <v>140</v>
       </c>
       <c r="B150" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C150" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D150" t="b">
         <v>0</v>
@@ -8525,10 +8528,10 @@
         <v>0</v>
       </c>
       <c r="H150" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="I150" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="J150" t="b">
         <v>1</v>
@@ -8539,10 +8542,10 @@
         <v>140</v>
       </c>
       <c r="B151" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C151" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D151" t="b">
         <v>0</v>
@@ -8557,10 +8560,10 @@
         <v>0</v>
       </c>
       <c r="H151" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="J151" t="b">
         <v>1</v>
@@ -8571,10 +8574,10 @@
         <v>140</v>
       </c>
       <c r="B152" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C152" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D152" t="b">
         <v>0</v>
@@ -8589,16 +8592,13 @@
         <v>0</v>
       </c>
       <c r="H152" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="J152" t="b">
         <v>1</v>
-      </c>
-      <c r="K152" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="153" spans="1:12">
@@ -8606,10 +8606,10 @@
         <v>140</v>
       </c>
       <c r="B153" t="s">
-        <v>170</v>
+        <v>243</v>
       </c>
       <c r="C153" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="D153" t="b">
         <v>0</v>
@@ -8624,16 +8624,13 @@
         <v>0</v>
       </c>
       <c r="H153" t="s">
-        <v>69</v>
+        <v>384</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>441</v>
+        <v>518</v>
       </c>
       <c r="J153" t="b">
         <v>1</v>
-      </c>
-      <c r="K153" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="154" spans="1:12">
@@ -8641,10 +8638,10 @@
         <v>140</v>
       </c>
       <c r="B154" t="s">
-        <v>171</v>
+        <v>244</v>
       </c>
       <c r="C154" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D154" t="b">
         <v>0</v>
@@ -8659,13 +8656,16 @@
         <v>0</v>
       </c>
       <c r="H154" t="s">
-        <v>310</v>
+        <v>385</v>
       </c>
       <c r="I154" s="2" t="s">
-        <v>442</v>
+        <v>519</v>
       </c>
       <c r="J154" t="b">
         <v>1</v>
+      </c>
+      <c r="K154" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="155" spans="1:12">
@@ -8673,10 +8673,10 @@
         <v>140</v>
       </c>
       <c r="B155" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C155" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D155" t="b">
         <v>0</v>
@@ -8691,16 +8691,16 @@
         <v>0</v>
       </c>
       <c r="H155" t="s">
-        <v>311</v>
+        <v>69</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J155" t="b">
         <v>1</v>
       </c>
-      <c r="L155" t="s">
-        <v>171</v>
+      <c r="K155" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="156" spans="1:12">
@@ -8708,16 +8708,16 @@
         <v>140</v>
       </c>
       <c r="B156" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C156" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D156" t="b">
         <v>0</v>
       </c>
       <c r="E156" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F156" t="b">
         <v>0</v>
@@ -8726,16 +8726,13 @@
         <v>0</v>
       </c>
       <c r="H156" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J156" t="b">
         <v>1</v>
-      </c>
-      <c r="L156" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="157" spans="1:12">
@@ -8743,16 +8740,16 @@
         <v>140</v>
       </c>
       <c r="B157" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C157" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D157" t="b">
         <v>0</v>
       </c>
       <c r="E157" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F157" t="b">
         <v>0</v>
@@ -8761,10 +8758,10 @@
         <v>0</v>
       </c>
       <c r="H157" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J157" t="b">
         <v>1</v>
@@ -8778,7 +8775,7 @@
         <v>140</v>
       </c>
       <c r="B158" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C158" t="s">
         <v>283</v>
@@ -8787,7 +8784,7 @@
         <v>0</v>
       </c>
       <c r="E158" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F158" t="b">
         <v>0</v>
@@ -8796,10 +8793,10 @@
         <v>0</v>
       </c>
       <c r="H158" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I158" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="J158" t="b">
         <v>1</v>
@@ -8813,7 +8810,7 @@
         <v>140</v>
       </c>
       <c r="B159" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C159" t="s">
         <v>274</v>
@@ -8822,7 +8819,7 @@
         <v>0</v>
       </c>
       <c r="E159" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F159" t="b">
         <v>0</v>
@@ -8831,10 +8828,10 @@
         <v>0</v>
       </c>
       <c r="H159" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J159" t="b">
         <v>1</v>
@@ -8845,19 +8842,19 @@
     </row>
     <row r="160" spans="1:12">
       <c r="A160" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B160" t="s">
-        <v>245</v>
+        <v>175</v>
       </c>
       <c r="C160" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="D160" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E160" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F160" t="b">
         <v>0</v>
@@ -8866,24 +8863,27 @@
         <v>0</v>
       </c>
       <c r="H160" t="s">
-        <v>386</v>
+        <v>314</v>
       </c>
       <c r="I160" s="2" t="s">
-        <v>520</v>
+        <v>446</v>
       </c>
       <c r="J160" t="b">
         <v>1</v>
+      </c>
+      <c r="L160" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="161" spans="1:12">
       <c r="A161" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B161" t="s">
-        <v>246</v>
+        <v>176</v>
       </c>
       <c r="C161" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D161" t="b">
         <v>0</v>
@@ -8898,16 +8898,16 @@
         <v>0</v>
       </c>
       <c r="H161" t="s">
-        <v>373</v>
+        <v>315</v>
       </c>
       <c r="I161" s="2" t="s">
-        <v>506</v>
+        <v>447</v>
       </c>
       <c r="J161" t="b">
         <v>1</v>
       </c>
-      <c r="K161" t="s">
-        <v>140</v>
+      <c r="L161" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="162" spans="1:12">
@@ -8915,16 +8915,16 @@
         <v>141</v>
       </c>
       <c r="B162" t="s">
-        <v>188</v>
+        <v>245</v>
       </c>
       <c r="C162" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D162" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E162" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F162" t="b">
         <v>0</v>
@@ -8933,16 +8933,13 @@
         <v>0</v>
       </c>
       <c r="H162" t="s">
-        <v>285</v>
+        <v>386</v>
       </c>
       <c r="I162" s="2" t="s">
-        <v>415</v>
+        <v>520</v>
       </c>
       <c r="J162" t="b">
         <v>1</v>
-      </c>
-      <c r="K162" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="163" spans="1:12">
@@ -8950,7 +8947,7 @@
         <v>141</v>
       </c>
       <c r="B163" t="s">
-        <v>168</v>
+        <v>246</v>
       </c>
       <c r="C163" t="s">
         <v>276</v>
@@ -8968,16 +8965,16 @@
         <v>0</v>
       </c>
       <c r="H163" t="s">
-        <v>309</v>
+        <v>373</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>439</v>
+        <v>507</v>
       </c>
       <c r="J163" t="b">
         <v>1</v>
       </c>
       <c r="K163" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="164" spans="1:12">
@@ -8985,10 +8982,10 @@
         <v>141</v>
       </c>
       <c r="B164" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="C164" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D164" t="b">
         <v>0</v>
@@ -9003,16 +9000,16 @@
         <v>0</v>
       </c>
       <c r="H164" t="s">
-        <v>66</v>
+        <v>285</v>
       </c>
       <c r="I164" s="2" t="s">
-        <v>440</v>
+        <v>415</v>
       </c>
       <c r="J164" t="b">
         <v>1</v>
       </c>
       <c r="K164" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="165" spans="1:12">
@@ -9020,10 +9017,10 @@
         <v>141</v>
       </c>
       <c r="B165" t="s">
-        <v>247</v>
+        <v>168</v>
       </c>
       <c r="C165" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D165" t="b">
         <v>0</v>
@@ -9038,13 +9035,16 @@
         <v>0</v>
       </c>
       <c r="H165" t="s">
-        <v>387</v>
+        <v>309</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>521</v>
+        <v>439</v>
       </c>
       <c r="J165" t="b">
         <v>1</v>
+      </c>
+      <c r="K165" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="166" spans="1:12">
@@ -9052,10 +9052,10 @@
         <v>141</v>
       </c>
       <c r="B166" t="s">
-        <v>248</v>
+        <v>169</v>
       </c>
       <c r="C166" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D166" t="b">
         <v>0</v>
@@ -9070,13 +9070,16 @@
         <v>0</v>
       </c>
       <c r="H166" t="s">
-        <v>388</v>
+        <v>66</v>
       </c>
       <c r="I166" s="2" t="s">
-        <v>522</v>
+        <v>440</v>
       </c>
       <c r="J166" t="b">
         <v>1</v>
+      </c>
+      <c r="K166" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="167" spans="1:12">
@@ -9084,7 +9087,7 @@
         <v>141</v>
       </c>
       <c r="B167" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C167" t="s">
         <v>274</v>
@@ -9102,10 +9105,10 @@
         <v>0</v>
       </c>
       <c r="H167" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="J167" t="b">
         <v>1</v>
@@ -9116,10 +9119,10 @@
         <v>141</v>
       </c>
       <c r="B168" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C168" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D168" t="b">
         <v>0</v>
@@ -9134,10 +9137,10 @@
         <v>0</v>
       </c>
       <c r="H168" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I168" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="J168" t="b">
         <v>1</v>
@@ -9148,7 +9151,7 @@
         <v>141</v>
       </c>
       <c r="B169" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C169" t="s">
         <v>274</v>
@@ -9166,10 +9169,10 @@
         <v>0</v>
       </c>
       <c r="H169" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I169" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="J169" t="b">
         <v>1</v>
@@ -9180,10 +9183,10 @@
         <v>141</v>
       </c>
       <c r="B170" t="s">
-        <v>30</v>
+        <v>250</v>
       </c>
       <c r="C170" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D170" t="b">
         <v>0</v>
@@ -9198,16 +9201,13 @@
         <v>0</v>
       </c>
       <c r="H170" t="s">
-        <v>81</v>
+        <v>390</v>
       </c>
       <c r="I170" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="J170" t="b">
         <v>1</v>
-      </c>
-      <c r="K170" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="171" spans="1:12">
@@ -9215,10 +9215,10 @@
         <v>141</v>
       </c>
       <c r="B171" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C171" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="D171" t="b">
         <v>0</v>
@@ -9233,10 +9233,10 @@
         <v>0</v>
       </c>
       <c r="H171" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I171" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="J171" t="b">
         <v>1</v>
@@ -9247,10 +9247,10 @@
         <v>141</v>
       </c>
       <c r="B172" t="s">
-        <v>253</v>
+        <v>30</v>
       </c>
       <c r="C172" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D172" t="b">
         <v>0</v>
@@ -9265,13 +9265,16 @@
         <v>0</v>
       </c>
       <c r="H172" t="s">
-        <v>304</v>
+        <v>81</v>
       </c>
       <c r="I172" s="2" t="s">
-        <v>434</v>
+        <v>526</v>
       </c>
       <c r="J172" t="b">
         <v>1</v>
+      </c>
+      <c r="K172" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="173" spans="1:12">
@@ -9279,10 +9282,10 @@
         <v>141</v>
       </c>
       <c r="B173" t="s">
-        <v>170</v>
+        <v>252</v>
       </c>
       <c r="C173" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D173" t="b">
         <v>0</v>
@@ -9297,16 +9300,13 @@
         <v>0</v>
       </c>
       <c r="H173" t="s">
-        <v>69</v>
+        <v>392</v>
       </c>
       <c r="I173" s="2" t="s">
-        <v>441</v>
+        <v>527</v>
       </c>
       <c r="J173" t="b">
         <v>1</v>
-      </c>
-      <c r="K173" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="174" spans="1:12">
@@ -9314,10 +9314,10 @@
         <v>141</v>
       </c>
       <c r="B174" t="s">
-        <v>171</v>
+        <v>253</v>
       </c>
       <c r="C174" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D174" t="b">
         <v>0</v>
@@ -9332,10 +9332,10 @@
         <v>0</v>
       </c>
       <c r="H174" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="I174" s="2" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="J174" t="b">
         <v>1</v>
@@ -9346,10 +9346,10 @@
         <v>141</v>
       </c>
       <c r="B175" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C175" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D175" t="b">
         <v>0</v>
@@ -9364,16 +9364,16 @@
         <v>0</v>
       </c>
       <c r="H175" t="s">
-        <v>311</v>
+        <v>69</v>
       </c>
       <c r="I175" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J175" t="b">
         <v>1</v>
       </c>
-      <c r="L175" t="s">
-        <v>171</v>
+      <c r="K175" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="176" spans="1:12">
@@ -9381,16 +9381,16 @@
         <v>141</v>
       </c>
       <c r="B176" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C176" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D176" t="b">
         <v>0</v>
       </c>
       <c r="E176" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F176" t="b">
         <v>0</v>
@@ -9399,16 +9399,13 @@
         <v>0</v>
       </c>
       <c r="H176" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I176" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J176" t="b">
         <v>1</v>
-      </c>
-      <c r="L176" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="177" spans="1:12">
@@ -9416,16 +9413,16 @@
         <v>141</v>
       </c>
       <c r="B177" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C177" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D177" t="b">
         <v>0</v>
       </c>
       <c r="E177" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F177" t="b">
         <v>0</v>
@@ -9434,10 +9431,10 @@
         <v>0</v>
       </c>
       <c r="H177" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I177" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J177" t="b">
         <v>1</v>
@@ -9451,7 +9448,7 @@
         <v>141</v>
       </c>
       <c r="B178" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C178" t="s">
         <v>283</v>
@@ -9460,7 +9457,7 @@
         <v>0</v>
       </c>
       <c r="E178" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F178" t="b">
         <v>0</v>
@@ -9469,10 +9466,10 @@
         <v>0</v>
       </c>
       <c r="H178" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I178" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="J178" t="b">
         <v>1</v>
@@ -9486,7 +9483,7 @@
         <v>141</v>
       </c>
       <c r="B179" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C179" t="s">
         <v>274</v>
@@ -9495,7 +9492,7 @@
         <v>0</v>
       </c>
       <c r="E179" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F179" t="b">
         <v>0</v>
@@ -9504,10 +9501,10 @@
         <v>0</v>
       </c>
       <c r="H179" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I179" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J179" t="b">
         <v>1</v>
@@ -9518,19 +9515,19 @@
     </row>
     <row r="180" spans="1:12">
       <c r="A180" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B180" t="s">
-        <v>254</v>
+        <v>175</v>
       </c>
       <c r="C180" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="D180" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E180" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F180" t="b">
         <v>0</v>
@@ -9539,21 +9536,24 @@
         <v>0</v>
       </c>
       <c r="H180" t="s">
-        <v>393</v>
+        <v>314</v>
       </c>
       <c r="I180" s="2" t="s">
-        <v>528</v>
+        <v>446</v>
       </c>
       <c r="J180" t="b">
         <v>1</v>
+      </c>
+      <c r="L180" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="181" spans="1:12">
       <c r="A181" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B181" t="s">
-        <v>255</v>
+        <v>176</v>
       </c>
       <c r="C181" t="s">
         <v>274</v>
@@ -9571,13 +9571,16 @@
         <v>0</v>
       </c>
       <c r="H181" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I181" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="J181" t="b">
         <v>1</v>
+      </c>
+      <c r="L181" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="182" spans="1:12">
@@ -9585,28 +9588,28 @@
         <v>142</v>
       </c>
       <c r="B182" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C182" t="s">
         <v>274</v>
       </c>
       <c r="D182" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E182" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F182" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G182" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H182" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I182" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J182" t="b">
         <v>1</v>
@@ -9617,10 +9620,10 @@
         <v>142</v>
       </c>
       <c r="B183" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C183" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D183" t="b">
         <v>0</v>
@@ -9635,10 +9638,10 @@
         <v>0</v>
       </c>
       <c r="H183" t="s">
-        <v>395</v>
+        <v>317</v>
       </c>
       <c r="I183" s="2" t="s">
-        <v>530</v>
+        <v>449</v>
       </c>
       <c r="J183" t="b">
         <v>1</v>
@@ -9649,7 +9652,7 @@
         <v>142</v>
       </c>
       <c r="B184" t="s">
-        <v>180</v>
+        <v>256</v>
       </c>
       <c r="C184" t="s">
         <v>274</v>
@@ -9661,16 +9664,16 @@
         <v>1</v>
       </c>
       <c r="F184" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G184" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H184" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I184" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="J184" t="b">
         <v>1</v>
@@ -9681,10 +9684,10 @@
         <v>142</v>
       </c>
       <c r="B185" t="s">
-        <v>161</v>
+        <v>257</v>
       </c>
       <c r="C185" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D185" t="b">
         <v>0</v>
@@ -9699,10 +9702,10 @@
         <v>0</v>
       </c>
       <c r="H185" t="s">
-        <v>302</v>
+        <v>395</v>
       </c>
       <c r="I185" s="2" t="s">
-        <v>432</v>
+        <v>530</v>
       </c>
       <c r="J185" t="b">
         <v>1</v>
@@ -9713,10 +9716,10 @@
         <v>142</v>
       </c>
       <c r="B186" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="C186" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D186" t="b">
         <v>0</v>
@@ -9731,10 +9734,10 @@
         <v>0</v>
       </c>
       <c r="H186" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I186" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="J186" t="b">
         <v>1</v>
@@ -9745,10 +9748,10 @@
         <v>142</v>
       </c>
       <c r="B187" t="s">
-        <v>258</v>
+        <v>161</v>
       </c>
       <c r="C187" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D187" t="b">
         <v>0</v>
@@ -9763,10 +9766,10 @@
         <v>0</v>
       </c>
       <c r="H187" t="s">
-        <v>398</v>
+        <v>302</v>
       </c>
       <c r="I187" s="2" t="s">
-        <v>533</v>
+        <v>432</v>
       </c>
       <c r="J187" t="b">
         <v>1</v>
@@ -9777,10 +9780,10 @@
         <v>142</v>
       </c>
       <c r="B188" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C188" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D188" t="b">
         <v>0</v>
@@ -9795,10 +9798,10 @@
         <v>0</v>
       </c>
       <c r="H188" t="s">
-        <v>310</v>
+        <v>397</v>
       </c>
       <c r="I188" s="2" t="s">
-        <v>442</v>
+        <v>532</v>
       </c>
       <c r="J188" t="b">
         <v>1</v>
@@ -9809,10 +9812,10 @@
         <v>142</v>
       </c>
       <c r="B189" t="s">
-        <v>172</v>
+        <v>258</v>
       </c>
       <c r="C189" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D189" t="b">
         <v>0</v>
@@ -9827,16 +9830,13 @@
         <v>0</v>
       </c>
       <c r="H189" t="s">
-        <v>311</v>
+        <v>398</v>
       </c>
       <c r="I189" s="2" t="s">
-        <v>443</v>
+        <v>533</v>
       </c>
       <c r="J189" t="b">
         <v>1</v>
-      </c>
-      <c r="L189" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="190" spans="1:12">
@@ -9844,16 +9844,16 @@
         <v>142</v>
       </c>
       <c r="B190" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C190" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D190" t="b">
         <v>0</v>
       </c>
       <c r="E190" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F190" t="b">
         <v>0</v>
@@ -9862,16 +9862,13 @@
         <v>0</v>
       </c>
       <c r="H190" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I190" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J190" t="b">
         <v>1</v>
-      </c>
-      <c r="L190" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="191" spans="1:12">
@@ -9879,16 +9876,16 @@
         <v>142</v>
       </c>
       <c r="B191" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C191" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D191" t="b">
         <v>0</v>
       </c>
       <c r="E191" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F191" t="b">
         <v>0</v>
@@ -9897,10 +9894,10 @@
         <v>0</v>
       </c>
       <c r="H191" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I191" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J191" t="b">
         <v>1</v>
@@ -9914,7 +9911,7 @@
         <v>142</v>
       </c>
       <c r="B192" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C192" t="s">
         <v>283</v>
@@ -9923,7 +9920,7 @@
         <v>0</v>
       </c>
       <c r="E192" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F192" t="b">
         <v>0</v>
@@ -9932,10 +9929,10 @@
         <v>0</v>
       </c>
       <c r="H192" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I192" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="J192" t="b">
         <v>1</v>
@@ -9949,7 +9946,7 @@
         <v>142</v>
       </c>
       <c r="B193" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C193" t="s">
         <v>274</v>
@@ -9958,7 +9955,7 @@
         <v>0</v>
       </c>
       <c r="E193" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F193" t="b">
         <v>0</v>
@@ -9967,10 +9964,10 @@
         <v>0</v>
       </c>
       <c r="H193" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I193" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J193" t="b">
         <v>1</v>
@@ -9981,42 +9978,45 @@
     </row>
     <row r="194" spans="1:12">
       <c r="A194" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B194" t="s">
-        <v>259</v>
+        <v>175</v>
       </c>
       <c r="C194" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="D194" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E194" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F194" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G194" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H194" t="s">
-        <v>399</v>
+        <v>314</v>
       </c>
       <c r="I194" s="2" t="s">
-        <v>534</v>
+        <v>446</v>
       </c>
       <c r="J194" t="b">
         <v>1</v>
+      </c>
+      <c r="L194" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="195" spans="1:12">
       <c r="A195" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B195" t="s">
-        <v>260</v>
+        <v>176</v>
       </c>
       <c r="C195" t="s">
         <v>274</v>
@@ -10034,13 +10034,16 @@
         <v>0</v>
       </c>
       <c r="H195" t="s">
-        <v>400</v>
+        <v>315</v>
       </c>
       <c r="I195" s="2" t="s">
-        <v>535</v>
+        <v>447</v>
       </c>
       <c r="J195" t="b">
         <v>1</v>
+      </c>
+      <c r="L195" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="196" spans="1:12">
@@ -10048,28 +10051,28 @@
         <v>143</v>
       </c>
       <c r="B196" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C196" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D196" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E196" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F196" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G196" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H196" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I196" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="J196" t="b">
         <v>1</v>
@@ -10080,7 +10083,7 @@
         <v>143</v>
       </c>
       <c r="B197" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C197" t="s">
         <v>274</v>
@@ -10098,10 +10101,10 @@
         <v>0</v>
       </c>
       <c r="H197" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I197" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J197" t="b">
         <v>1</v>
@@ -10112,10 +10115,10 @@
         <v>143</v>
       </c>
       <c r="B198" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C198" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D198" t="b">
         <v>0</v>
@@ -10130,10 +10133,10 @@
         <v>0</v>
       </c>
       <c r="H198" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I198" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J198" t="b">
         <v>1</v>
@@ -10144,10 +10147,10 @@
         <v>143</v>
       </c>
       <c r="B199" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C199" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D199" t="b">
         <v>0</v>
@@ -10162,10 +10165,10 @@
         <v>0</v>
       </c>
       <c r="H199" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="I199" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J199" t="b">
         <v>1</v>
@@ -10173,31 +10176,31 @@
     </row>
     <row r="200" spans="1:12">
       <c r="A200" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B200" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C200" t="s">
         <v>274</v>
       </c>
       <c r="D200" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E200" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F200" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G200" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H200" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I200" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="J200" t="b">
         <v>1</v>
@@ -10205,10 +10208,10 @@
     </row>
     <row r="201" spans="1:12">
       <c r="A201" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B201" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C201" t="s">
         <v>282</v>
@@ -10226,10 +10229,10 @@
         <v>0</v>
       </c>
       <c r="H201" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="I201" s="2" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="J201" t="b">
         <v>1</v>
@@ -10240,28 +10243,28 @@
         <v>144</v>
       </c>
       <c r="B202" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C202" t="s">
         <v>274</v>
       </c>
       <c r="D202" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E202" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F202" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G202" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H202" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I202" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J202" t="b">
         <v>1</v>
@@ -10272,10 +10275,10 @@
         <v>144</v>
       </c>
       <c r="B203" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C203" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D203" t="b">
         <v>0</v>
@@ -10290,10 +10293,10 @@
         <v>0</v>
       </c>
       <c r="H203" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="I203" s="2" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="J203" t="b">
         <v>1</v>
@@ -10304,10 +10307,10 @@
         <v>144</v>
       </c>
       <c r="B204" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C204" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D204" t="b">
         <v>0</v>
@@ -10322,10 +10325,10 @@
         <v>0</v>
       </c>
       <c r="H204" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I204" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J204" t="b">
         <v>1</v>
@@ -10333,19 +10336,19 @@
     </row>
     <row r="205" spans="1:12">
       <c r="A205" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B205" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C205" t="s">
         <v>274</v>
       </c>
       <c r="D205" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E205" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F205" t="b">
         <v>0</v>
@@ -10354,10 +10357,10 @@
         <v>0</v>
       </c>
       <c r="H205" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="I205" s="2" t="s">
-        <v>528</v>
+        <v>542</v>
       </c>
       <c r="J205" t="b">
         <v>1</v>
@@ -10365,13 +10368,13 @@
     </row>
     <row r="206" spans="1:12">
       <c r="A206" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B206" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="C206" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="D206" t="b">
         <v>0</v>
@@ -10380,16 +10383,16 @@
         <v>1</v>
       </c>
       <c r="F206" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G206" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H206" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="I206" s="2" t="s">
-        <v>529</v>
+        <v>543</v>
       </c>
       <c r="J206" t="b">
         <v>1</v>
@@ -10400,16 +10403,16 @@
         <v>145</v>
       </c>
       <c r="B207" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="C207" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D207" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E207" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F207" t="b">
         <v>0</v>
@@ -10418,10 +10421,10 @@
         <v>0</v>
       </c>
       <c r="H207" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="I207" s="2" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="J207" t="b">
         <v>1</v>
@@ -10432,10 +10435,10 @@
         <v>145</v>
       </c>
       <c r="B208" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="C208" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="D208" t="b">
         <v>0</v>
@@ -10444,16 +10447,16 @@
         <v>1</v>
       </c>
       <c r="F208" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G208" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H208" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="I208" s="2" t="s">
-        <v>544</v>
+        <v>529</v>
       </c>
       <c r="J208" t="b">
         <v>1</v>
@@ -10464,10 +10467,10 @@
         <v>145</v>
       </c>
       <c r="B209" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="C209" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D209" t="b">
         <v>0</v>
@@ -10482,10 +10485,10 @@
         <v>0</v>
       </c>
       <c r="H209" t="s">
-        <v>313</v>
+        <v>409</v>
       </c>
       <c r="I209" s="2" t="s">
-        <v>445</v>
+        <v>536</v>
       </c>
       <c r="J209" t="b">
         <v>1</v>
@@ -10496,10 +10499,10 @@
         <v>145</v>
       </c>
       <c r="B210" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C210" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="D210" t="b">
         <v>0</v>
@@ -10514,10 +10517,10 @@
         <v>0</v>
       </c>
       <c r="H210" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I210" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="J210" t="b">
         <v>1</v>
@@ -10528,7 +10531,7 @@
         <v>145</v>
       </c>
       <c r="B211" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C211" t="s">
         <v>274</v>
@@ -10546,10 +10549,10 @@
         <v>0</v>
       </c>
       <c r="H211" t="s">
-        <v>412</v>
+        <v>313</v>
       </c>
       <c r="I211" s="2" t="s">
-        <v>546</v>
+        <v>445</v>
       </c>
       <c r="J211" t="b">
         <v>1</v>
@@ -10560,10 +10563,10 @@
         <v>145</v>
       </c>
       <c r="B212" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C212" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D212" t="b">
         <v>0</v>
@@ -10578,10 +10581,10 @@
         <v>0</v>
       </c>
       <c r="H212" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="I212" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="J212" t="b">
         <v>1</v>
@@ -10589,19 +10592,19 @@
     </row>
     <row r="213" spans="1:10">
       <c r="A213" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B213" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C213" t="s">
         <v>274</v>
       </c>
       <c r="D213" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E213" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F213" t="b">
         <v>0</v>
@@ -10610,10 +10613,10 @@
         <v>0</v>
       </c>
       <c r="H213" t="s">
-        <v>393</v>
+        <v>412</v>
       </c>
       <c r="I213" s="2" t="s">
-        <v>528</v>
+        <v>546</v>
       </c>
       <c r="J213" t="b">
         <v>1</v>
@@ -10621,13 +10624,13 @@
     </row>
     <row r="214" spans="1:10">
       <c r="A214" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B214" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="C214" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D214" t="b">
         <v>0</v>
@@ -10636,16 +10639,16 @@
         <v>1</v>
       </c>
       <c r="F214" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G214" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H214" t="s">
-        <v>394</v>
+        <v>413</v>
       </c>
       <c r="I214" s="2" t="s">
-        <v>529</v>
+        <v>547</v>
       </c>
       <c r="J214" t="b">
         <v>1</v>
@@ -10656,16 +10659,16 @@
         <v>146</v>
       </c>
       <c r="B215" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="C215" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D215" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E215" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F215" t="b">
         <v>0</v>
@@ -10674,10 +10677,10 @@
         <v>0</v>
       </c>
       <c r="H215" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="I215" s="2" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="J215" t="b">
         <v>1</v>
@@ -10688,7 +10691,7 @@
         <v>146</v>
       </c>
       <c r="B216" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="C216" t="s">
         <v>274</v>
@@ -10700,16 +10703,16 @@
         <v>1</v>
       </c>
       <c r="F216" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G216" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H216" t="s">
-        <v>414</v>
+        <v>394</v>
       </c>
       <c r="I216" s="2" t="s">
-        <v>548</v>
+        <v>529</v>
       </c>
       <c r="J216" t="b">
         <v>1</v>
@@ -10720,10 +10723,10 @@
         <v>146</v>
       </c>
       <c r="B217" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C217" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D217" t="b">
         <v>0</v>
@@ -10738,10 +10741,10 @@
         <v>0</v>
       </c>
       <c r="H217" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="I217" s="2" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="J217" t="b">
         <v>1</v>
@@ -10749,31 +10752,31 @@
     </row>
     <row r="218" spans="1:10">
       <c r="A218" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="B218" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="C218" t="s">
         <v>274</v>
       </c>
       <c r="D218" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E218" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F218" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G218" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H218" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="I218" s="2" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="J218" t="b">
         <v>1</v>
@@ -10781,13 +10784,13 @@
     </row>
     <row r="219" spans="1:10">
       <c r="A219" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="B219" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="C219" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D219" t="b">
         <v>0</v>
@@ -10802,10 +10805,10 @@
         <v>0</v>
       </c>
       <c r="H219" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="I219" s="2" t="s">
-        <v>536</v>
+        <v>543</v>
       </c>
       <c r="J219" t="b">
         <v>1</v>
@@ -10816,28 +10819,28 @@
         <v>132</v>
       </c>
       <c r="B220" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C220" t="s">
         <v>274</v>
       </c>
       <c r="D220" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E220" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F220" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G220" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H220" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I220" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J220" t="b">
         <v>1</v>
@@ -10848,10 +10851,10 @@
         <v>132</v>
       </c>
       <c r="B221" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C221" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D221" t="b">
         <v>0</v>
@@ -10866,10 +10869,10 @@
         <v>0</v>
       </c>
       <c r="H221" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="I221" s="2" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="J221" t="b">
         <v>1</v>
@@ -10880,10 +10883,10 @@
         <v>132</v>
       </c>
       <c r="B222" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C222" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D222" t="b">
         <v>0</v>
@@ -10898,10 +10901,10 @@
         <v>0</v>
       </c>
       <c r="H222" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I222" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J222" t="b">
         <v>1</v>
@@ -10909,10 +10912,10 @@
     </row>
     <row r="223" spans="1:10">
       <c r="A223" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B223" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C223" t="s">
         <v>274</v>
@@ -10924,16 +10927,16 @@
         <v>1</v>
       </c>
       <c r="F223" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G223" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H223" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I223" s="2" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="J223" t="b">
         <v>1</v>
@@ -10941,13 +10944,13 @@
     </row>
     <row r="224" spans="1:10">
       <c r="A224" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B224" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="C224" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D224" t="b">
         <v>0</v>
@@ -10962,10 +10965,10 @@
         <v>0</v>
       </c>
       <c r="H224" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="I224" s="2" t="s">
-        <v>536</v>
+        <v>543</v>
       </c>
       <c r="J224" t="b">
         <v>1</v>
@@ -10976,7 +10979,7 @@
         <v>133</v>
       </c>
       <c r="B225" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C225" t="s">
         <v>274</v>
@@ -10988,16 +10991,16 @@
         <v>1</v>
       </c>
       <c r="F225" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G225" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H225" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I225" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J225" t="b">
         <v>1</v>
@@ -11008,16 +11011,16 @@
         <v>133</v>
       </c>
       <c r="B226" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C226" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="D226" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E226" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F226" t="b">
         <v>0</v>
@@ -11026,10 +11029,10 @@
         <v>0</v>
       </c>
       <c r="H226" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="I226" s="2" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="J226" t="b">
         <v>1</v>
@@ -11040,30 +11043,94 @@
         <v>133</v>
       </c>
       <c r="B227" t="s">
+        <v>265</v>
+      </c>
+      <c r="C227" t="s">
+        <v>274</v>
+      </c>
+      <c r="D227" t="b">
+        <v>0</v>
+      </c>
+      <c r="E227" t="b">
+        <v>1</v>
+      </c>
+      <c r="F227" t="b">
+        <v>0</v>
+      </c>
+      <c r="G227" t="b">
+        <v>0</v>
+      </c>
+      <c r="H227" t="s">
+        <v>406</v>
+      </c>
+      <c r="I227" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="J227" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10">
+      <c r="A228" t="s">
+        <v>133</v>
+      </c>
+      <c r="B228" t="s">
+        <v>259</v>
+      </c>
+      <c r="C228" t="s">
+        <v>274</v>
+      </c>
+      <c r="D228" t="b">
+        <v>1</v>
+      </c>
+      <c r="E228" t="b">
+        <v>0</v>
+      </c>
+      <c r="F228" t="b">
+        <v>0</v>
+      </c>
+      <c r="G228" t="b">
+        <v>0</v>
+      </c>
+      <c r="H228" t="s">
+        <v>407</v>
+      </c>
+      <c r="I228" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="J228" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10">
+      <c r="A229" t="s">
+        <v>133</v>
+      </c>
+      <c r="B229" t="s">
         <v>266</v>
       </c>
-      <c r="C227" t="s">
+      <c r="C229" t="s">
         <v>284</v>
       </c>
-      <c r="D227" t="b">
-        <v>0</v>
-      </c>
-      <c r="E227" t="b">
-        <v>1</v>
-      </c>
-      <c r="F227" t="b">
-        <v>0</v>
-      </c>
-      <c r="G227" t="b">
-        <v>0</v>
-      </c>
-      <c r="H227" t="s">
+      <c r="D229" t="b">
+        <v>0</v>
+      </c>
+      <c r="E229" t="b">
+        <v>1</v>
+      </c>
+      <c r="F229" t="b">
+        <v>0</v>
+      </c>
+      <c r="G229" t="b">
+        <v>0</v>
+      </c>
+      <c r="H229" t="s">
         <v>408</v>
       </c>
-      <c r="I227" s="2" t="s">
+      <c r="I229" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="J227" t="b">
+      <c r="J229" t="b">
         <v>1</v>
       </c>
     </row>
@@ -11186,9 +11253,9 @@
     <hyperlink ref="I118" r:id="rId115" location="wasUpdatedBy"/>
     <hyperlink ref="I119" r:id="rId116"/>
     <hyperlink ref="I120" r:id="rId117"/>
-    <hyperlink ref="I121" r:id="rId118" location="AFRL_0000010"/>
+    <hyperlink ref="I121" r:id="rId118"/>
     <hyperlink ref="I122" r:id="rId119"/>
-    <hyperlink ref="I123" r:id="rId120"/>
+    <hyperlink ref="I123" r:id="rId120" location="AFRL_0000010"/>
     <hyperlink ref="I124" r:id="rId121"/>
     <hyperlink ref="I125" r:id="rId122"/>
     <hyperlink ref="I126" r:id="rId123"/>
@@ -11201,9 +11268,9 @@
     <hyperlink ref="I133" r:id="rId130"/>
     <hyperlink ref="I134" r:id="rId131"/>
     <hyperlink ref="I135" r:id="rId132"/>
-    <hyperlink ref="I136" r:id="rId133" location="wasUpdatedBy"/>
+    <hyperlink ref="I136" r:id="rId133"/>
     <hyperlink ref="I137" r:id="rId134"/>
-    <hyperlink ref="I138" r:id="rId135"/>
+    <hyperlink ref="I138" r:id="rId135" location="wasUpdatedBy"/>
     <hyperlink ref="I139" r:id="rId136"/>
     <hyperlink ref="I140" r:id="rId137"/>
     <hyperlink ref="I141" r:id="rId138"/>
@@ -11224,9 +11291,9 @@
     <hyperlink ref="I156" r:id="rId153"/>
     <hyperlink ref="I157" r:id="rId154"/>
     <hyperlink ref="I158" r:id="rId155"/>
-    <hyperlink ref="I159" r:id="rId156" location="wasUpdatedBy"/>
+    <hyperlink ref="I159" r:id="rId156"/>
     <hyperlink ref="I160" r:id="rId157"/>
-    <hyperlink ref="I161" r:id="rId158"/>
+    <hyperlink ref="I161" r:id="rId158" location="wasUpdatedBy"/>
     <hyperlink ref="I162" r:id="rId159"/>
     <hyperlink ref="I163" r:id="rId160"/>
     <hyperlink ref="I164" r:id="rId161"/>
@@ -11244,9 +11311,9 @@
     <hyperlink ref="I176" r:id="rId173"/>
     <hyperlink ref="I177" r:id="rId174"/>
     <hyperlink ref="I178" r:id="rId175"/>
-    <hyperlink ref="I179" r:id="rId176" location="wasUpdatedBy"/>
+    <hyperlink ref="I179" r:id="rId176"/>
     <hyperlink ref="I180" r:id="rId177"/>
-    <hyperlink ref="I181" r:id="rId178"/>
+    <hyperlink ref="I181" r:id="rId178" location="wasUpdatedBy"/>
     <hyperlink ref="I182" r:id="rId179"/>
     <hyperlink ref="I183" r:id="rId180"/>
     <hyperlink ref="I184" r:id="rId181"/>
@@ -11258,9 +11325,9 @@
     <hyperlink ref="I190" r:id="rId187"/>
     <hyperlink ref="I191" r:id="rId188"/>
     <hyperlink ref="I192" r:id="rId189"/>
-    <hyperlink ref="I193" r:id="rId190" location="wasUpdatedBy"/>
+    <hyperlink ref="I193" r:id="rId190"/>
     <hyperlink ref="I194" r:id="rId191"/>
-    <hyperlink ref="I195" r:id="rId192"/>
+    <hyperlink ref="I195" r:id="rId192" location="wasUpdatedBy"/>
     <hyperlink ref="I196" r:id="rId193"/>
     <hyperlink ref="I197" r:id="rId194"/>
     <hyperlink ref="I198" r:id="rId195"/>
@@ -11293,6 +11360,8 @@
     <hyperlink ref="I225" r:id="rId222"/>
     <hyperlink ref="I226" r:id="rId223"/>
     <hyperlink ref="I227" r:id="rId224"/>
+    <hyperlink ref="I228" r:id="rId225"/>
+    <hyperlink ref="I229" r:id="rId226"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11408,13 +11477,13 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B6" t="s">
         <v>601</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D6" t="s">
         <v>745</v>
@@ -11628,13 +11697,13 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B17" t="s">
         <v>612</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D17" t="s">
         <v>751</v>
@@ -12008,13 +12077,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B36" t="s">
         <v>631</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D36" t="s">
         <v>755</v>
@@ -12028,13 +12097,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B37" t="s">
         <v>632</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="D37" t="s">
         <v>755</v>
@@ -12328,13 +12397,13 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B52" t="s">
         <v>647</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D52" t="s">
         <v>755</v>
@@ -12528,13 +12597,13 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B62" t="s">
         <v>657</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D62" t="s">
         <v>755</v>
@@ -12788,13 +12857,13 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="B75" t="s">
         <v>670</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="D75" t="s">
         <v>755</v>
@@ -13048,13 +13117,13 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B88" t="s">
         <v>683</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D88" t="s">
         <v>755</v>
@@ -13288,13 +13357,13 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B100" t="s">
         <v>695</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D100" t="s">
         <v>755</v>
@@ -14088,13 +14157,13 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B140" t="s">
         <v>735</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D140" t="s">
         <v>763</v>
@@ -14128,13 +14197,13 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B142" t="s">
         <v>737</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D142" t="s">
         <v>765</v>

</xml_diff>